<commit_message>
Estructuración en carpetas y agregado de rutas
</commit_message>
<xml_diff>
--- a/Sorteo Estructuras.xlsx
+++ b/Sorteo Estructuras.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140"/>
   </bookViews>
   <sheets>
     <sheet name=" AuxGrafBolillas " sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="64">
   <si>
     <t>AuxGrafBolillaFechaSorteo</t>
   </si>
@@ -218,105 +218,6 @@
   </si>
   <si>
     <t>N</t>
-  </si>
-  <si>
-    <t>CREATE TABLE [dbo].[AuxGrafBolillas](</t>
-  </si>
-  <si>
-    <t>[AuxGrafBolillaFechaSorteo] [datetime] NOT NULL,</t>
-  </si>
-  <si>
-    <t>[AuxGrafBolillaNumero] [int] NOT NULL,</t>
-  </si>
-  <si>
-    <t>[AuxGrafBolillaPosicion] [smallint] NULL,</t>
-  </si>
-  <si>
-    <t>[AuxGrafBolillaGruposFav] [varchar](max) NULL,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRIMARY KEY CLUSTERED </t>
-  </si>
-  <si>
-    <t>(</t>
-  </si>
-  <si>
-    <t>[AuxGrafBolillaFechaSorteo] ASC,</t>
-  </si>
-  <si>
-    <t>[AuxGrafBolillaNumero] ASC</t>
-  </si>
-  <si>
-    <t>CREATE TABLE [dbo].[AuxGrafGanadores](</t>
-  </si>
-  <si>
-    <t>[AuxGrafGanadorFechaSorteo] [datetime] NOT NULL,</t>
-  </si>
-  <si>
-    <t>[AuxGrafGanadorGrupoCodigo] [decimal](10, 0) NOT NULL,</t>
-  </si>
-  <si>
-    <t>[AuxGrafGanadorBolillaNumero] [int] NOT NULL,</t>
-  </si>
-  <si>
-    <t>[AuxGrafGanadorGrupoNombre] [char](30) NULL,</t>
-  </si>
-  <si>
-    <t>[AuxGrafGanadorTipoAdj] [char](1) NULL,</t>
-  </si>
-  <si>
-    <t>[AuxGrafGanadorCuotasOferta] [int] NULL,</t>
-  </si>
-  <si>
-    <t>[AuxGrafGanadorDeptoNombre] [char](30) NULL,</t>
-  </si>
-  <si>
-    <t>[AuxGrafGanadorFechaSorteo] ASC,</t>
-  </si>
-  <si>
-    <t>[AuxGrafGanadorGrupoCodigo] ASC,</t>
-  </si>
-  <si>
-    <t>[AuxGrafGanadorBolillaNumero] ASC</t>
-  </si>
-  <si>
-    <t>CREATE TABLE [dbo].[AuxGrafLicitaciones](</t>
-  </si>
-  <si>
-    <t>[AuxGrafLicFechaSorteo] [datetime] NOT NULL,</t>
-  </si>
-  <si>
-    <t>[AuxGrafLicGrupoCodigo] [decimal](10, 0) NOT NULL,</t>
-  </si>
-  <si>
-    <t>[AuxGrafLicBolillaNumero] [int] NOT NULL,</t>
-  </si>
-  <si>
-    <t>[AuxGrafLicGrupoNombre] [char](30) NOT NULL,</t>
-  </si>
-  <si>
-    <t>[AuxGrafLicBolillaPosicion] [smallint] NOT NULL,</t>
-  </si>
-  <si>
-    <t>[AuxGrafLicTipoAdj] [char](1) NOT NULL,</t>
-  </si>
-  <si>
-    <t>[AuxGrafLicOfertaTope] [smallint] NOT NULL,</t>
-  </si>
-  <si>
-    <t>[AuxGrafLicOfertaLibre] [smallint] NOT NULL,</t>
-  </si>
-  <si>
-    <t>[AuxGrafLicEstadoCodigo] [char](1) NOT NULL,</t>
-  </si>
-  <si>
-    <t>[AuxGrafLicFechaSorteo] ASC,</t>
-  </si>
-  <si>
-    <t>[AuxGrafLicGrupoCodigo] ASC,</t>
-  </si>
-  <si>
-    <t>[AuxGrafLicBolillaNumero] ASC</t>
   </si>
 </sst>
 </file>
@@ -668,21 +569,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L401"/>
+  <dimension ref="A1:D401"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L12" sqref="K9:L12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="81.5546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="33" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="43.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -696,7 +599,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -707,7 +610,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -718,7 +621,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -728,11 +631,8 @@
       <c r="C4">
         <v>126</v>
       </c>
-      <c r="K4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -742,11 +642,8 @@
       <c r="C5">
         <v>340</v>
       </c>
-      <c r="L5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -756,11 +653,8 @@
       <c r="C6">
         <v>242</v>
       </c>
-      <c r="L6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -770,11 +664,8 @@
       <c r="C7">
         <v>237</v>
       </c>
-      <c r="L7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -784,11 +675,8 @@
       <c r="C8">
         <v>196</v>
       </c>
-      <c r="L8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -798,11 +686,8 @@
       <c r="C9">
         <v>207</v>
       </c>
-      <c r="K9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -815,11 +700,8 @@
       <c r="D10" t="s">
         <v>5</v>
       </c>
-      <c r="K10" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -829,11 +711,8 @@
       <c r="C11">
         <v>211</v>
       </c>
-      <c r="L11" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -843,11 +722,8 @@
       <c r="C12">
         <v>333</v>
       </c>
-      <c r="L12" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -858,7 +734,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -869,7 +745,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -880,7 +756,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -5151,15 +5027,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K4" sqref="K4:L16"/>
+      <selection activeCell="K1" sqref="K1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -5182,7 +5058,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -5205,7 +5081,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -5228,7 +5104,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -5250,11 +5126,8 @@
       <c r="G4" t="s">
         <v>25</v>
       </c>
-      <c r="K4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -5276,11 +5149,8 @@
       <c r="G5" t="s">
         <v>28</v>
       </c>
-      <c r="L5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -5302,11 +5172,8 @@
       <c r="G6" t="s">
         <v>25</v>
       </c>
-      <c r="L6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -5328,11 +5195,8 @@
       <c r="G7" t="s">
         <v>30</v>
       </c>
-      <c r="L7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -5354,11 +5218,8 @@
       <c r="G8" t="s">
         <v>25</v>
       </c>
-      <c r="L8" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -5380,11 +5241,8 @@
       <c r="G9" t="s">
         <v>25</v>
       </c>
-      <c r="L9" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -5406,11 +5264,8 @@
       <c r="G10" t="s">
         <v>25</v>
       </c>
-      <c r="L10" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -5432,11 +5287,8 @@
       <c r="G11" t="s">
         <v>23</v>
       </c>
-      <c r="L11" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -5458,11 +5310,8 @@
       <c r="G12" t="s">
         <v>35</v>
       </c>
-      <c r="K12" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -5484,11 +5333,8 @@
       <c r="G13" t="s">
         <v>37</v>
       </c>
-      <c r="K13" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -5510,11 +5356,8 @@
       <c r="G14" t="s">
         <v>38</v>
       </c>
-      <c r="L14" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -5536,11 +5379,8 @@
       <c r="G15" t="s">
         <v>40</v>
       </c>
-      <c r="L15" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -5561,9 +5401,6 @@
       </c>
       <c r="G16" t="s">
         <v>42</v>
-      </c>
-      <c r="L16" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -5895,15 +5732,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M52"/>
+  <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5:M19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>53</v>
       </c>
@@ -5932,7 +5769,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -5961,7 +5798,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -5990,7 +5827,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -6019,7 +5856,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -6047,11 +5884,8 @@
       <c r="I5" t="s">
         <v>63</v>
       </c>
-      <c r="L5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -6079,11 +5913,8 @@
       <c r="I6" t="s">
         <v>27</v>
       </c>
-      <c r="M6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -6111,11 +5942,8 @@
       <c r="I7" t="s">
         <v>63</v>
       </c>
-      <c r="M7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -6143,11 +5971,8 @@
       <c r="I8" t="s">
         <v>27</v>
       </c>
-      <c r="M8" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -6175,11 +6000,8 @@
       <c r="I9" t="s">
         <v>63</v>
       </c>
-      <c r="M9" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -6207,11 +6029,8 @@
       <c r="I10" t="s">
         <v>27</v>
       </c>
-      <c r="M10" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -6239,11 +6058,8 @@
       <c r="I11" t="s">
         <v>63</v>
       </c>
-      <c r="M11" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -6271,11 +6087,8 @@
       <c r="I12" t="s">
         <v>63</v>
       </c>
-      <c r="M12" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -6303,11 +6116,8 @@
       <c r="I13" t="s">
         <v>63</v>
       </c>
-      <c r="M13" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -6335,11 +6145,8 @@
       <c r="I14" t="s">
         <v>63</v>
       </c>
-      <c r="M14" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -6367,11 +6174,8 @@
       <c r="I15" t="s">
         <v>27</v>
       </c>
-      <c r="L15" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -6399,11 +6203,8 @@
       <c r="I16" t="s">
         <v>63</v>
       </c>
-      <c r="L16" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -6431,11 +6232,8 @@
       <c r="I17" t="s">
         <v>63</v>
       </c>
-      <c r="M17" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -6463,11 +6261,8 @@
       <c r="I18" t="s">
         <v>63</v>
       </c>
-      <c r="M18" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -6495,11 +6290,8 @@
       <c r="I19" t="s">
         <v>63</v>
       </c>
-      <c r="M19" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -6528,7 +6320,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -6557,7 +6349,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -6586,7 +6378,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -6615,7 +6407,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>4</v>
       </c>
@@ -6644,7 +6436,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>4</v>
       </c>
@@ -6673,7 +6465,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -6702,7 +6494,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>4</v>
       </c>
@@ -6731,7 +6523,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -6760,7 +6552,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -6789,7 +6581,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>4</v>
       </c>
@@ -6818,7 +6610,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>4</v>
       </c>
@@ -6847,7 +6639,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>4</v>
       </c>

</xml_diff>